<commit_message>
Edits to paper and data dictionary
</commit_message>
<xml_diff>
--- a/Final project/Data/Final dataset/data dictionary.xlsx
+++ b/Final project/Data/Final dataset/data dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marjoriecrowell/Documents/Data management/Data management assignments/Final project/Final dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marjoriecrowell/Documents/Data management/Data management assignments/Final project/Data/Final dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B40F174-0DF7-6044-8517-96E99F81F3E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C18F2FF-29DA-764E-B9C5-5C7E745832F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="460" windowWidth="27640" windowHeight="16540" xr2:uid="{2BCBF3C8-F131-EB44-9641-6BA8C55F3F78}"/>
+    <workbookView xWindow="10340" yWindow="460" windowWidth="20780" windowHeight="16540" xr2:uid="{2BCBF3C8-F131-EB44-9641-6BA8C55F3F78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="135">
   <si>
     <t>Variable</t>
   </si>
@@ -42,32 +42,458 @@
     <t>Values</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Year of data</t>
   </si>
   <si>
-    <t>numberproviders</t>
-  </si>
-  <si>
     <t>state_fullname</t>
   </si>
   <si>
-    <t>numbercpcs</t>
-  </si>
-  <si>
-    <t>numberabortions</t>
-  </si>
-  <si>
     <t>Indicator/ measure</t>
+  </si>
+  <si>
+    <t>number_providers</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>number_cpcs</t>
+  </si>
+  <si>
+    <t>number_abortions</t>
+  </si>
+  <si>
+    <t>any_gest_limit_str</t>
+  </si>
+  <si>
+    <t>ultrasound_required_str</t>
+  </si>
+  <si>
+    <t>asc_requirement_str</t>
+  </si>
+  <si>
+    <t>pre_roe_ban_str</t>
+  </si>
+  <si>
+    <t>want_to_limit_str</t>
+  </si>
+  <si>
+    <t>protects_right_str</t>
+  </si>
+  <si>
+    <t>hyde_str</t>
+  </si>
+  <si>
+    <t>more_than_hyde_str</t>
+  </si>
+  <si>
+    <t>parental_consent_str</t>
+  </si>
+  <si>
+    <t>partial_birth_ban_str</t>
+  </si>
+  <si>
+    <t>medicaid_expanded_str</t>
+  </si>
+  <si>
+    <t>uninsured_2010</t>
+  </si>
+  <si>
+    <t>uninsured_2015</t>
+  </si>
+  <si>
+    <t>uninsured_change_201015</t>
+  </si>
+  <si>
+    <t>state_pop</t>
+  </si>
+  <si>
+    <t>vote2016_str</t>
+  </si>
+  <si>
+    <t>vote2012_str</t>
+  </si>
+  <si>
+    <t>waiting_yn</t>
+  </si>
+  <si>
+    <t>ultrasound_yn</t>
+  </si>
+  <si>
+    <t>any_gest_limit_yn</t>
+  </si>
+  <si>
+    <t>asc_requirement_yn</t>
+  </si>
+  <si>
+    <t>pre_roe_ban_yn</t>
+  </si>
+  <si>
+    <t>protects_right_yn</t>
+  </si>
+  <si>
+    <t>hyde_yn</t>
+  </si>
+  <si>
+    <t>more_than_hyde_yn</t>
+  </si>
+  <si>
+    <t>partial_birth_ban_yn</t>
+  </si>
+  <si>
+    <t>republican2012_yn</t>
+  </si>
+  <si>
+    <t>republican2016_yn</t>
+  </si>
+  <si>
+    <t>medicaid_expanded_yn</t>
+  </si>
+  <si>
+    <t>want_to_limit_yn</t>
+  </si>
+  <si>
+    <t>restrictive_policy_yn</t>
+  </si>
+  <si>
+    <t>composite_regulations</t>
+  </si>
+  <si>
+    <t>composite_providers</t>
+  </si>
+  <si>
+    <t>composite_regulations_protective</t>
+  </si>
+  <si>
+    <t>composite_parients</t>
+  </si>
+  <si>
+    <t>number of abortion providers</t>
+  </si>
+  <si>
+    <t>Guttmacher Institute: https://data.guttmacher.org/states/table?state=AL+AK+AZ+AR+CA+CO+CT+DE+DC+FL+GA+HI+ID+IL+IN+IA+KS+KY+LA+ME+MD+MA+MI+MN+MS+MO+MT+NE+NV+NH+NJ+NM+NY+NC+ND+OH+OK+OR+PA+RI+SC+SD+TN+TX+UT+VT+VA+WA+WV+WI+WY&amp;topics=57&amp;dataset=data</t>
+  </si>
+  <si>
+    <t>1-152</t>
+  </si>
+  <si>
+    <t>state abbreviation</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>state full name</t>
+  </si>
+  <si>
+    <t>number of crisis pregnancy centers</t>
+  </si>
+  <si>
+    <t>Reproaction: https://reproaction.org/fakeclinicdatabase/</t>
+  </si>
+  <si>
+    <t>3-180</t>
+  </si>
+  <si>
+    <t>number of abortions provided (occurrence)</t>
+  </si>
+  <si>
+    <t>Guttmacher Institute: https://data.guttmacher.org/states/table?state=AL+AK+AZ+AR+CA+CO+CT+DE+DC+FL+GA+HI+ID+IL+IN+IA+KS+KY+LA+ME+MD+MA+MI+MN+MS+MO+MT+NE+NV+NH+NJ+NM+NY+NC+ND+OH+OK+OR+PA+RI+SC+SD+TN+TX+UT+VT+VA+WA+WV+WI+WY&amp;topics=66&amp;dataset=data</t>
+  </si>
+  <si>
+    <t>120-157,350</t>
+  </si>
+  <si>
+    <t>Data type</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>"AK" - "WY"</t>
+  </si>
+  <si>
+    <t>"Alabama" - "Wyoming"</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>No
+Yes</t>
+  </si>
+  <si>
+    <t>No
+Yes
+Yes; Policy not in effect</t>
+  </si>
+  <si>
+    <t>whether state regulation prohibits abortion past any point in gestation</t>
+  </si>
+  <si>
+    <t>whether state regulation requires abortion facilities to adhere to ambulatory surgical center requirements</t>
+  </si>
+  <si>
+    <t>whether state law retains a law from prior to the Roe v. Wade decision which restricts abortion (not enforceable)</t>
+  </si>
+  <si>
+    <t>whether state policy expresses an intent to limit abortion as much as possible under the law (not enforceable)</t>
+  </si>
+  <si>
+    <t>whether state law protects the right to abortion</t>
+  </si>
+  <si>
+    <t>whether state Medciaid policy follows the federal standard under the Hyde amendment (does not allow Medicaid funding for abortion except in case of life endangerment, rape, or incest)</t>
+  </si>
+  <si>
+    <t>whether state Medicaid policy will alllow Medicaid funding for abortion that goes above Hyde standard</t>
+  </si>
+  <si>
+    <t>whether state has elected to expand Medicaid eligibility under Affordable Care Act</t>
+  </si>
+  <si>
+    <t>percent of people in state without insurance in 2010</t>
+  </si>
+  <si>
+    <t>percent of people in state without insurance in 2015</t>
+  </si>
+  <si>
+    <t>change in uninsured rate between 2010 and 2015</t>
+  </si>
+  <si>
+    <t>total population in state</t>
+  </si>
+  <si>
+    <t>Federal Elections Commission</t>
+  </si>
+  <si>
+    <t>compiled dataset, source: Federal Elections Commission</t>
+  </si>
+  <si>
+    <t>U.S. Department of Health and Human Services: https://www.kaggle.com/hhs/health-insurance</t>
+  </si>
+  <si>
+    <t>Kaiser Family Foundation: https://www.kff.org/health-reform/state-indicator/state-activity-around-expanding-medicaid-under-the-affordable-care-act/?currentTimeframe=0&amp;sortModel=%7B%22colId%22:%22Location%22,%22sort%22:%22asc%22%7D</t>
+  </si>
+  <si>
+    <t>"Adopted" 
+"Not Adopted"</t>
+  </si>
+  <si>
+    <t>min: 4.4
+max: 23.7</t>
+  </si>
+  <si>
+    <t>min: 2.8
+max: 17.1</t>
+  </si>
+  <si>
+    <t>min: -10.3
+max: -1.6</t>
+  </si>
+  <si>
+    <t>min: 563,300
+max: 3.87e+07</t>
+  </si>
+  <si>
+    <t>"D"
+"R"</t>
+  </si>
+  <si>
+    <t>party affiliation of presidential candidate voters in state overwhelmingly chose in 2016 presidential election</t>
+  </si>
+  <si>
+    <t>party affiliation of presidential candidate voters in state overwhelmingly chose in 2012 presidential election</t>
+  </si>
+  <si>
+    <t>KFF datastet (uses Guttmacher data): https://www.kff.org/womens-health-policy/state-indicator/gestational-limit-abortions/?currentTimeframe=0&amp;sortModel=%7B%22colId%22:%22Location%22,%22sort%22:%22asc%22%7D</t>
+  </si>
+  <si>
+    <t>as of January 1, 2019</t>
+  </si>
+  <si>
+    <t>0 = "No"
+1 = "Yes"</t>
+  </si>
+  <si>
+    <t>waiting_period_str</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1="Yes" 
+0="No", "Enjoined; policy not in effect", "Policy temporary enjoined; policy not in effect"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Yes" 
+"No"
+"Enjoined; policy not in effect" "Policy temporary enjoined; policy not in effect"</t>
+  </si>
+  <si>
+    <t>as of October 1, 2018</t>
+  </si>
+  <si>
+    <t>KFF datastet (uses Guttmacher data): https://www.kff.org/womens-health-policy/state-indicator/mandatory-waiting-periods/?currentTimeframe=0&amp;sortModel=%7B%22colId%22:%22Location%22,%22sort%22:%22asc%22%7D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">whether state regulation requires a person seeking abortion to receive information on accessing ultrasound services, or that person undergo an ultrasound before an abortion. </t>
+  </si>
+  <si>
+    <t>as of April 1, 2017</t>
+  </si>
+  <si>
+    <t>KFF dataset (uses Guttmacher data): https://www.kff.org/womens-health-policy/state-indicator/ultrasound-requirements/?currentTimeframe=0&amp;sortModel=%7B%22colId%22:%22Location%22,%22sort%22:%22asc%22%7D</t>
+  </si>
+  <si>
+    <t>as of October 4, 2018</t>
+  </si>
+  <si>
+    <t>KFF dataset (uses Guttmacher data): https://www.kff.org/womens-health-policy/state-indicator/regulations-on-facilities-and-clinicians-providing-abortions/?currentTimeframe=0&amp;sortModel=%7B%22colId%22:%22Location%22,%22sort%22:%22asc%22%7D</t>
+  </si>
+  <si>
+    <t>0 = "No"
+1 = "Yes"; "Yes; Policy not in effect"</t>
+  </si>
+  <si>
+    <t>KFF dataset (uses Guttmacher data): https://www.kff.org/womens-health-policy/state-indicator/state-policies-protecting-or-restricting-legal-status-of-abortion/?currentTimeframe=0&amp;sortModel=%7B%22colId%22:%22Location%22,%22sort%22:%22asc%22%7D</t>
+  </si>
+  <si>
+    <t>recode of pre_roe_ban_yn and want_to_limit_yn</t>
+  </si>
+  <si>
+    <t>0 if want_to_limit_yn and pre_roe_ban_yn BOTH = "No"
+1 if want_to_limit_yn OR pre_roe_ban_yn OR BOTH = "Yes"</t>
+  </si>
+  <si>
+    <t>as of November 16, 2018</t>
+  </si>
+  <si>
+    <t>KFF dataset (uses Guttmacher data): https://www.kff.org/medicaid/state-indicator/abortion-under-medicaid/?currentTimeframe=0&amp;sortModel=%7B%22colId%22:%22Location%22,%22sort%22:%22asc%22%7D</t>
+  </si>
+  <si>
+    <t>recode of vote2012_str</t>
+  </si>
+  <si>
+    <t>recode of vote2016_str</t>
+  </si>
+  <si>
+    <t>0 if vote2012_str = "D"
+1 if vote2012_str = "R"</t>
+  </si>
+  <si>
+    <t>0 if vote2016_str = "D"
+1 if vote2016_str = "R"</t>
+  </si>
+  <si>
+    <t>0 = "Not Adopted"
+1 = "Adopted"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">whether state has enacted a ban on so-called "Partial-birth abortion" </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+"So-called "partial birth abortion" is not a medical term. These bans may be interpreted to prohibit certain abortion procedures including the D&amp;X procedure (dilation and extraction) used in a small share of second trimester abortions. These bans may also be interpreted to apply to the more common second trimester D&amp;E procedure (dilation and evacuation), which has led to controversy about the bans' scope."</t>
+    </r>
+  </si>
+  <si>
+    <t>as of June 1, 2018</t>
+  </si>
+  <si>
+    <t>KFF dataset (uses Guttmacher data): https://www.kff.org/womens-health-policy/state-indicator/partial-birth-abortion-bans/?currentTimeframe=0&amp;sortModel=%7B%22colId%22:%22Location%22,%22sort%22:%22asc%22%7D</t>
+  </si>
+  <si>
+    <t>0 = "No"; "Enjoined or not enforced"
+1 = "Yes"</t>
+  </si>
+  <si>
+    <t>"No"
+"Enjoined or not enforced"
+"Yes"</t>
+  </si>
+  <si>
+    <t>state requires parental consent or notification for minors seeking abortion services</t>
+  </si>
+  <si>
+    <t>KFF dataset (uses Guttmacher data): https://www.kff.org/womens-health-policy/state-indicator/parental-consentnotification/?currentTimeframe=0&amp;sortModel=%7B%22colId%22:%22Location%22,%22sort%22:%22asc%22%7D</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1= "Consent enforced"; "Notification and consent enforced"
+"Notification enforced"
+0 = "No Law" 
+ "Consent enjoined or not enforced"
+"Notification enjoined or not enforced"
+"Consent and notification temporarily enjoined"
+		</t>
+  </si>
+  <si>
+    <t>"Consent enforced" "Notification and consent enforced"
+"Notification enforced"
+ "No Law" 
+ "Consent enjoined or not enforced"
+"Notification enjoined or not enforced"
+"Consent and notification temporarily enjoined"</t>
+  </si>
+  <si>
+    <t>KFF dataset (uses Census Bureau's American Community Survey): https://www.kff.org/other/state-indicator/total-residents/?currentTimeframe=0&amp;sortModel=%7B%22colId%22:%22Location%22,%22sort%22:%22asc%22%7D</t>
+  </si>
+  <si>
+    <t>recode: sum of values of (parental_consent_yn + partial_birth_ban_yn + hyde_yn
++ restrictive_policy_yn + asc_requirement_yn + any_gest_limit_yn + ultrasound_yn + waiting_yn)</t>
+  </si>
+  <si>
+    <t>recode: sum of values of (partial_birth_ban_yn + asc_requirement_yn)</t>
+  </si>
+  <si>
+    <t>recode: sum of values of (parental_consent_yn + hyde_yn + any_gest_limit_yn + ultrasound_yn + waiting_yn)</t>
+  </si>
+  <si>
+    <t>recode: sum of values of (parental_consent_yn + partial_birth_ban_yn + hyde_yn + restrictive_policy_yn + asc_requirement_yn + any_gest_limit_yn + ultrasound_yn + waiting_yn) minus values of (more_than_hyde_yn + protects_right_yn)</t>
+  </si>
+  <si>
+    <t>as of April 2019</t>
+  </si>
+  <si>
+    <t>2017-2019 (depends on individual measures)</t>
+  </si>
+  <si>
+    <t>KFF datasets using Guttmacher data</t>
+  </si>
+  <si>
+    <t>min: 0
+max: 8</t>
+  </si>
+  <si>
+    <t>min: 0
+max: 2</t>
+  </si>
+  <si>
+    <t>min: 0
+max: 5</t>
+  </si>
+  <si>
+    <t>min: -2
+max: 8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,6 +504,21 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -110,13 +551,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,20 +882,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF1C0A2-A006-6B42-82B3-DC1A64D40781}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -454,40 +905,863 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2014</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2014</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="187" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2010</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2012</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="221" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2012</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D44" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
reorganized code and data files
</commit_message>
<xml_diff>
--- a/Final project/Data/Final dataset/data dictionary.xlsx
+++ b/Final project/Data/Final dataset/data dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marjoriecrowell/Documents/Data management/Data management assignments/Final project/Data/Final dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB8234A-7521-8644-87E4-43631B87E9FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5BD877-DB75-ED45-B485-EE561B189902}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10340" yWindow="460" windowWidth="20780" windowHeight="16540" xr2:uid="{2BCBF3C8-F131-EB44-9641-6BA8C55F3F78}"/>
+    <workbookView xWindow="10000" yWindow="460" windowWidth="20780" windowHeight="16540" xr2:uid="{2BCBF3C8-F131-EB44-9641-6BA8C55F3F78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -923,8 +923,8 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>